<commit_message>
Aether Light Basic functioning
</commit_message>
<xml_diff>
--- a/Code/STM32f439ZIT6U Aether Light/Aether Light BOM.xlsx
+++ b/Code/STM32f439ZIT6U Aether Light/Aether Light BOM.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nanodyn-my.sharepoint.com/personal/nicholas_nanodyn_co_za/Documents/Desktop/GIT repository/Waveform-generator/Code/STM32f439ZIT6U Aether Light/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_946C2C74AF38D79B2497E595C702F02375465F98" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4FC910C4-83E9-4613-81CA-A1B16CCD83C4}"/>
+  <bookViews>
+    <workbookView xWindow="-10620" yWindow="5985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -52,9 +72,6 @@
     <t>STM</t>
   </si>
   <si>
-    <t>Raspberry Pi 4 Model B</t>
-  </si>
-  <si>
     <t>Raspberry Pi</t>
   </si>
   <si>
@@ -70,9 +87,6 @@
     <t>Made in house</t>
   </si>
   <si>
-    <t xml:space="preserve">Solenoid- 2V025-08 </t>
-  </si>
-  <si>
     <t>Airtac</t>
   </si>
   <si>
@@ -98,37 +112,128 @@
   </si>
   <si>
     <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>Price per item</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4 Model B 8GB</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>497-18153-ND</t>
+  </si>
+  <si>
+    <t>PI4-8GB</t>
+  </si>
+  <si>
+    <t>XGZP6847A010KPGPN</t>
+  </si>
+  <si>
+    <t>PBS-33B</t>
+  </si>
+  <si>
+    <t>P135</t>
+  </si>
+  <si>
+    <t>LRS-100-12</t>
+  </si>
+  <si>
+    <t>RS components</t>
+  </si>
+  <si>
+    <t>A9S65240</t>
+  </si>
+  <si>
+    <t>XL4016</t>
+  </si>
+  <si>
+    <t>2ACK-12V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t>JF-1039B</t>
+  </si>
+  <si>
+    <t>This excludes the cost of the piping and wiring</t>
+  </si>
+  <si>
+    <t>PH128800TDD4-ZFAD1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;R&quot;#,##0.00;[Red]\-&quot;R&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="10">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Docs-Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -136,7 +241,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -146,171 +251,274 @@
     </fill>
   </fills>
   <borders count="13">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
+  <cellXfs count="43">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -500,213 +708,361 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.43"/>
-    <col customWidth="1" min="3" max="3" width="18.14"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="D3" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="33">
+        <v>530.1</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="D4" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="39">
+        <v>398.85</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="36">
+        <v>135</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
+      <c r="D7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="33">
+        <v>500</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="36">
+        <v>1298</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="16">
-        <v>2.0</v>
+      <c r="B10" s="15">
+        <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="D10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="33">
+        <v>139</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="39">
+        <v>132</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="D12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="36">
+        <v>153</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="B14" s="10">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="B15" s="12">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="E17" s="33">
+        <v>1910.3</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B18" s="16">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="39">
+        <v>39</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="E19" s="36">
+        <v>22</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="D20" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="42">
+        <f>SUM(E3:E19)</f>
+        <v>5257.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="D22" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>